<commit_message>
Bg: fix tests, async => done()
</commit_message>
<xml_diff>
--- a/tests/mockData/addResultsDataTableDuplicate.xlsx
+++ b/tests/mockData/addResultsDataTableDuplicate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Documents/Github/v9-bears-team-21/tests/mockData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{372F747E-5F0A-F542-8DBE-9BA8A33A3840}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{670DBA5C-CD5D-784B-994F-E565C8DB071F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{83A0CDA4-EF9A-9B4C-8749-8981E60F4772}"/>
   </bookViews>
@@ -45,12 +45,6 @@
     <t>grade</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>jamsgra</t>
-  </si>
-  <si>
     <t>Maths</t>
   </si>
   <si>
@@ -67,13 +61,19 @@
   </si>
   <si>
     <t>20/100</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>jamsgra.doey@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +88,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,7 +119,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +437,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,7 +452,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -469,7 +475,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>2010</v>
@@ -478,21 +484,21 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
+      <c r="A3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B3">
         <v>2010</v>
@@ -501,16 +507,16 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>